<commit_message>
case 3 borrowing book works
</commit_message>
<xml_diff>
--- a/resources/Library.xlsx
+++ b/resources/Library.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\libraryhhs\resources\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="59">
   <si>
     <t>Title</t>
   </si>
@@ -186,12 +186,40 @@
   </si>
   <si>
     <t>Inventory</t>
+  </si>
+  <si>
+    <t>Ego Is The Enemy</t>
+  </si>
+  <si>
+    <t>Ryan Holiday</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>9781591847816</t>
+  </si>
+  <si>
+    <t>Portfolio, Penguin</t>
+  </si>
+  <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>Non-fiction</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -540,7 +568,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C00CA1DD-83D4-4E24-A179-F9689E3BB369}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
@@ -548,147 +576,147 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.140625" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="39.140625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="31.85546875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="59.0"/>
+    <col min="4" max="4" customWidth="true" width="14.7109375"/>
+    <col min="5" max="5" customWidth="true" width="27.28515625"/>
+    <col min="6" max="6" customWidth="true" width="21.140625"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="17.5703125"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.7109375"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14.28515625"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.28515625"/>
+    <col min="11" max="11" customWidth="true" width="10.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" t="s" s="0">
         <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>15</v>
       </c>
       <c r="D2" s="1">
         <v>9780446310789</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>24</v>
       </c>
       <c r="F2" s="3">
         <v>1988</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="0">
         <v>10</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="0">
         <v>11</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>16</v>
       </c>
       <c r="D3" s="1">
         <v>9780590353427</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>25</v>
       </c>
       <c r="F3" s="3">
         <v>1997</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="0">
         <v>6</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="0">
         <v>26</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>17</v>
       </c>
       <c r="D4" s="1">
         <v>9780316769488</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>26</v>
       </c>
       <c r="F4" s="3">
         <v>1991</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="0">
         <v>5</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="0">
         <v>1</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="0">
         <v>8</v>
       </c>
     </row>
@@ -696,202 +724,202 @@
       <c r="A5" s="2">
         <v>1984</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>18</v>
       </c>
       <c r="D5" s="1">
         <v>9780451524935</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>27</v>
       </c>
       <c r="F5" s="3">
         <v>1961</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="0">
         <v>8</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="0">
         <v>1</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>19</v>
       </c>
       <c r="D6" s="1">
         <v>9780743273565</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>28</v>
       </c>
       <c r="F6" s="3">
         <v>2004</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="0">
         <v>9</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="0">
         <v>30</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>23</v>
       </c>
       <c r="D7" s="1">
         <v>9780345339706</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" t="s" s="0">
         <v>29</v>
       </c>
       <c r="F7" s="3">
         <v>1986</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="0">
         <v>7</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="0">
         <v>12</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>20</v>
       </c>
       <c r="D8" s="1">
         <v>9780547928227</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" t="s" s="0">
         <v>30</v>
       </c>
       <c r="F8" s="3">
         <v>2012</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="0">
         <v>9</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="0">
         <v>18</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>21</v>
       </c>
       <c r="D9" s="1">
         <v>9780345391803</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" t="s" s="0">
         <v>31</v>
       </c>
       <c r="F9" s="3">
         <v>1995</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="0">
         <v>8</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="0">
         <v>17</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>22</v>
       </c>
       <c r="D10" s="1">
         <v>9781613820122</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" t="s" s="0">
         <v>32</v>
       </c>
       <c r="F10" s="3">
         <v>2011</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="0">
         <v>5</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="0">
         <v>19</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" t="s" s="0">
         <v>39</v>
       </c>
       <c r="D11" s="1">
@@ -900,49 +928,84 @@
       <c r="F11" s="3">
         <v>1946</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" t="s" s="0">
         <v>44</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" t="s" s="0">
         <v>46</v>
       </c>
       <c r="D12" s="1">
         <v>9781781257654</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" t="s" s="0">
         <v>47</v>
       </c>
       <c r="F12" s="3">
         <v>2016</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="0">
         <v>10</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="0">
         <v>18</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="K12">
-        <v>8</v>
+      <c r="K12" s="0" t="n">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="E13" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="F13" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="G13" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="H13" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="I13" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="J13" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="K13" t="n" s="0">
+        <v>8.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>